<commit_message>
corrected the bug in stata do file. Now high income low risks. high education low risks.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corrM.xlsx
+++ b/WorkingFolder/Tables/corrM.xlsx
@@ -471,40 +471,40 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>-0.6308995147500133</v>
+        <v>-0.4739381494412931</v>
       </c>
       <c r="D2">
-        <v>0.009262429175671837</v>
+        <v>0.1382547059950641</v>
       </c>
       <c r="E2">
-        <v>0.03909911308846689</v>
+        <v>0.09155845137439581</v>
       </c>
       <c r="G2">
-        <v>-0.0272495615874394</v>
+        <v>0.03335360499461792</v>
       </c>
       <c r="H2">
-        <v>-0.3907610993612261</v>
+        <v>0.1328582935888218</v>
       </c>
       <c r="I2">
-        <v>0.08096266493471405</v>
+        <v>-0.07028726428208364</v>
       </c>
       <c r="J2">
-        <v>0.07723008918389183</v>
+        <v>0.06559350788852032</v>
       </c>
       <c r="K2">
-        <v>0.1510477846896381</v>
+        <v>0.07359892647541673</v>
       </c>
       <c r="L2">
-        <v>0.06790307946415082</v>
+        <v>-0.06826462012334182</v>
       </c>
       <c r="M2">
-        <v>0.07350566084732679</v>
+        <v>0.03826994240463905</v>
       </c>
       <c r="N2">
-        <v>-0.3952229613793843</v>
+        <v>0.05534716907154695</v>
       </c>
       <c r="O2">
-        <v>0.133508310383175</v>
+        <v>-0.008456246078771197</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -512,7 +512,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-0.6308995147500133</v>
+        <v>-0.4739381494412931</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -556,7 +556,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.009262429175671837</v>
+        <v>0.1382547059950641</v>
       </c>
       <c r="C4">
         <v>0.05832643982846182</v>
@@ -600,7 +600,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.03909911308846689</v>
+        <v>0.09155845137439581</v>
       </c>
       <c r="C5">
         <v>-0.0754838018301929</v>
@@ -649,7 +649,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-0.0272495615874394</v>
+        <v>0.03335360499461792</v>
       </c>
       <c r="C7">
         <v>-0.0631266661179027</v>
@@ -693,7 +693,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.3907610993612261</v>
+        <v>0.1328582935888218</v>
       </c>
       <c r="C8">
         <v>0.1050650681005624</v>
@@ -737,7 +737,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.08096266493471405</v>
+        <v>-0.07028726428208364</v>
       </c>
       <c r="C9">
         <v>0.09657169854192199</v>
@@ -781,7 +781,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.07723008918389183</v>
+        <v>0.06559350788852032</v>
       </c>
       <c r="C10">
         <v>-0.02109617420717148</v>
@@ -825,7 +825,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.1510477846896381</v>
+        <v>0.07359892647541673</v>
       </c>
       <c r="C11">
         <v>-0.03779534862855197</v>
@@ -869,7 +869,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.06790307946415082</v>
+        <v>-0.06826462012334182</v>
       </c>
       <c r="C12">
         <v>0.04802500255917358</v>
@@ -913,7 +913,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.07350566084732679</v>
+        <v>0.03826994240463905</v>
       </c>
       <c r="C13">
         <v>0.006474357331293395</v>
@@ -957,7 +957,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-0.3952229613793843</v>
+        <v>0.05534716907154695</v>
       </c>
       <c r="C14">
         <v>0.06839736194028714</v>
@@ -1001,7 +1001,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.133508310383175</v>
+        <v>-0.008456246078771197</v>
       </c>
       <c r="C15">
         <v>0.05532713645521843</v>

</xml_diff>

<commit_message>
counter cyclical perceived risks. negative correlation of realized wage growth and perceived risk.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corrM.xlsx
+++ b/WorkingFolder/Tables/corrM.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>sp500</t>
   </si>
   <si>
     <t>VIXCLS</t>
+  </si>
+  <si>
+    <t>he</t>
   </si>
   <si>
     <t>expMed</t>
@@ -413,13 +416,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,8 +465,11 @@
       <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,572 +477,658 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>-0.7047556261015829</v>
+        <v>-0.4739381494412931</v>
       </c>
       <c r="D2">
-        <v>-0.04743437747629582</v>
+        <v>0.01919449350673576</v>
       </c>
       <c r="E2">
-        <v>0.02275530254629318</v>
-      </c>
-      <c r="G2">
-        <v>0.01984950350403698</v>
+        <v>0.1353018484758965</v>
+      </c>
+      <c r="F2">
+        <v>0.09068930835106143</v>
       </c>
       <c r="H2">
-        <v>-0.07735816559944704</v>
+        <v>0.03676615276217467</v>
       </c>
       <c r="I2">
-        <v>-0.1403061574535686</v>
+        <v>0.1295600575368288</v>
       </c>
       <c r="J2">
-        <v>-0.04671663250852448</v>
+        <v>-0.0639152332538617</v>
       </c>
       <c r="K2">
-        <v>0.02676678503401862</v>
+        <v>0.05640457747579858</v>
       </c>
       <c r="L2">
-        <v>-0.07828834604569371</v>
+        <v>0.07053265861265146</v>
       </c>
       <c r="M2">
-        <v>0.004732017893733165</v>
+        <v>-0.07450578906792989</v>
       </c>
       <c r="N2">
-        <v>-0.08118141911519945</v>
+        <v>0.03265917347778867</v>
       </c>
       <c r="O2">
-        <v>-0.02673676715644199</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>0.05382833303964853</v>
+      </c>
+      <c r="P2">
+        <v>-0.009843459895422251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-0.7047556261015829</v>
+        <v>-0.4739381494412931</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
+        <v>0.1023066948649261</v>
+      </c>
+      <c r="E3">
         <v>0.07440478395551647</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>-0.06986646035450562</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>-0.06051795811232875</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.1143498427673656</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.09527665589281313</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>-0.01151755191354742</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>-0.02914244125909981</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>0.04876962339280161</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>0.01742559811962423</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>0.06934592894886464</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0.06306186227928907</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.04743437747629582</v>
+        <v>0.01919449350673576</v>
       </c>
       <c r="C4">
-        <v>0.07440478395551647</v>
+        <v>0.1023066948649261</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.3456618958283406</v>
-      </c>
-      <c r="G4">
-        <v>0.3269328383725711</v>
+        <v>0.0664357926112886</v>
+      </c>
+      <c r="F4">
+        <v>-0.1564425234255272</v>
       </c>
       <c r="H4">
-        <v>0.3958692142618715</v>
+        <v>-0.2202972830706263</v>
       </c>
       <c r="I4">
-        <v>0.03844707986648056</v>
+        <v>0.1483430455084005</v>
       </c>
       <c r="J4">
-        <v>0.8041894500608463</v>
+        <v>-0.2082208012276153</v>
       </c>
       <c r="K4">
-        <v>0.1418704476126033</v>
+        <v>-0.02102817223964968</v>
       </c>
       <c r="L4">
-        <v>-0.01463024890903251</v>
+        <v>-0.142443795964709</v>
       </c>
       <c r="M4">
-        <v>0.05679644052597838</v>
+        <v>0.1077856607014213</v>
       </c>
       <c r="N4">
-        <v>0.3661331865400339</v>
+        <v>-0.06144998064813029</v>
       </c>
       <c r="O4">
-        <v>0.04245051279411372</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+        <v>0.1362113189276979</v>
+      </c>
+      <c r="P4">
+        <v>-0.1364125383050702</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.02275530254629318</v>
+        <v>0.1353018484758965</v>
       </c>
       <c r="C5">
-        <v>-0.06986646035450562</v>
+        <v>0.07440478395551647</v>
       </c>
       <c r="D5">
+        <v>0.0664357926112886</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>0.3456618958283406</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0.952956949937701</v>
-      </c>
       <c r="H5">
-        <v>0.3616315137833193</v>
+        <v>0.3269328383725711</v>
       </c>
       <c r="I5">
-        <v>0.3244402953268535</v>
+        <v>0.3958692142618715</v>
       </c>
       <c r="J5">
-        <v>0.6315695168996384</v>
+        <v>0.03844707986648056</v>
       </c>
       <c r="K5">
-        <v>0.06432798670309411</v>
+        <v>0.8041894500608463</v>
       </c>
       <c r="L5">
-        <v>-0.09781173102871583</v>
+        <v>0.1418704476126033</v>
       </c>
       <c r="M5">
-        <v>-0.1980138146036305</v>
+        <v>-0.01463024890903251</v>
       </c>
       <c r="N5">
-        <v>0.4101233346279459</v>
+        <v>0.05679644052597838</v>
       </c>
       <c r="O5">
-        <v>0.09082176799679093</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+        <v>0.3661331865400339</v>
+      </c>
+      <c r="P5">
+        <v>0.04245051279411372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="B6">
+        <v>0.09068930835106143</v>
+      </c>
+      <c r="C6">
+        <v>-0.06986646035450562</v>
+      </c>
+      <c r="D6">
+        <v>-0.1564425234255272</v>
+      </c>
+      <c r="E6">
+        <v>0.3456618958283406</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0.952956949937701</v>
+      </c>
+      <c r="I6">
+        <v>0.3616315137833193</v>
+      </c>
+      <c r="J6">
+        <v>0.3244402953268535</v>
+      </c>
+      <c r="K6">
+        <v>0.6315695168996384</v>
+      </c>
+      <c r="L6">
+        <v>0.06432798670309411</v>
+      </c>
+      <c r="M6">
+        <v>-0.09781173102871583</v>
+      </c>
+      <c r="N6">
+        <v>-0.1980138146036305</v>
+      </c>
+      <c r="O6">
+        <v>0.4101233346279459</v>
+      </c>
+      <c r="P6">
+        <v>0.09082176799679093</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>0.01984950350403698</v>
-      </c>
-      <c r="C7">
-        <v>-0.06051795811232875</v>
-      </c>
-      <c r="D7">
-        <v>0.3269328383725711</v>
-      </c>
-      <c r="E7">
-        <v>0.952956949937701</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>0.3122748691730542</v>
-      </c>
-      <c r="I7">
-        <v>0.3819806403851467</v>
-      </c>
-      <c r="J7">
-        <v>0.6010659765620737</v>
-      </c>
-      <c r="K7">
-        <v>0.1802842195832685</v>
-      </c>
-      <c r="L7">
-        <v>-0.0427452430127298</v>
-      </c>
-      <c r="M7">
-        <v>-0.07627511032712242</v>
-      </c>
-      <c r="N7">
-        <v>0.3858841094161588</v>
-      </c>
-      <c r="O7">
-        <v>0.1521262490988143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.07735816559944704</v>
+        <v>0.03676615276217467</v>
       </c>
       <c r="C8">
-        <v>0.1143498427673656</v>
+        <v>-0.06051795811232875</v>
       </c>
       <c r="D8">
-        <v>0.3958692142618715</v>
+        <v>-0.2202972830706263</v>
       </c>
       <c r="E8">
-        <v>0.3616315137833193</v>
-      </c>
-      <c r="G8">
+        <v>0.3269328383725711</v>
+      </c>
+      <c r="F8">
+        <v>0.952956949937701</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>0.3122748691730542</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>-0.2083907738613129</v>
-      </c>
       <c r="J8">
-        <v>0.445985760966529</v>
+        <v>0.3819806403851467</v>
       </c>
       <c r="K8">
-        <v>-0.1506489769386493</v>
+        <v>0.6010659765620737</v>
       </c>
       <c r="L8">
-        <v>-0.3230280538554612</v>
+        <v>0.1802842195832685</v>
       </c>
       <c r="M8">
-        <v>-0.225486848726541</v>
+        <v>-0.0427452430127298</v>
       </c>
       <c r="N8">
-        <v>0.9082083413765707</v>
+        <v>-0.07627511032712242</v>
       </c>
       <c r="O8">
-        <v>-0.1723749541018063</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+        <v>0.3858841094161588</v>
+      </c>
+      <c r="P8">
+        <v>0.1521262490988143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-0.1403061574535686</v>
+        <v>0.1295600575368288</v>
       </c>
       <c r="C9">
-        <v>0.09527665589281313</v>
+        <v>0.1143498427673656</v>
       </c>
       <c r="D9">
-        <v>0.03844707986648056</v>
+        <v>0.1483430455084005</v>
       </c>
       <c r="E9">
-        <v>0.3244402953268535</v>
-      </c>
-      <c r="G9">
-        <v>0.3819806403851467</v>
+        <v>0.3958692142618715</v>
+      </c>
+      <c r="F9">
+        <v>0.3616315137833193</v>
       </c>
       <c r="H9">
+        <v>0.3122748691730542</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
         <v>-0.2083907738613129</v>
       </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>0.1987560697275382</v>
-      </c>
       <c r="K9">
-        <v>0.6522674128189277</v>
+        <v>0.445985760966529</v>
       </c>
       <c r="L9">
-        <v>0.114092003527871</v>
+        <v>-0.1506489769386493</v>
       </c>
       <c r="M9">
-        <v>0.4944986209532007</v>
+        <v>-0.3230280538554612</v>
       </c>
       <c r="N9">
-        <v>-0.1579486423221279</v>
+        <v>-0.225486848726541</v>
       </c>
       <c r="O9">
-        <v>0.7403132706269152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+        <v>0.9082083413765707</v>
+      </c>
+      <c r="P9">
+        <v>-0.1723749541018063</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-0.04671663250852448</v>
+        <v>-0.0639152332538617</v>
       </c>
       <c r="C10">
-        <v>-0.01151755191354742</v>
+        <v>0.09527665589281313</v>
       </c>
       <c r="D10">
-        <v>0.8041894500608463</v>
+        <v>-0.2082208012276153</v>
       </c>
       <c r="E10">
-        <v>0.6315695168996384</v>
-      </c>
-      <c r="G10">
-        <v>0.6010659765620737</v>
+        <v>0.03844707986648056</v>
+      </c>
+      <c r="F10">
+        <v>0.3244402953268535</v>
       </c>
       <c r="H10">
-        <v>0.445985760966529</v>
+        <v>0.3819806403851467</v>
       </c>
       <c r="I10">
+        <v>-0.2083907738613129</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
         <v>0.1987560697275382</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>0.2525430715716202</v>
-      </c>
       <c r="L10">
-        <v>-0.1349869902559086</v>
+        <v>0.6522674128189277</v>
       </c>
       <c r="M10">
-        <v>0.05601955201777537</v>
+        <v>0.114092003527871</v>
       </c>
       <c r="N10">
-        <v>0.5188514403663723</v>
+        <v>0.4944986209532007</v>
       </c>
       <c r="O10">
-        <v>0.1893413854013475</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+        <v>-0.1579486423221279</v>
+      </c>
+      <c r="P10">
+        <v>0.7403132706269152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.02676678503401862</v>
+        <v>0.05640457747579858</v>
       </c>
       <c r="C11">
-        <v>-0.02914244125909981</v>
+        <v>-0.01151755191354742</v>
       </c>
       <c r="D11">
-        <v>0.1418704476126033</v>
+        <v>-0.02102817223964968</v>
       </c>
       <c r="E11">
-        <v>0.06432798670309411</v>
-      </c>
-      <c r="G11">
-        <v>0.1802842195832685</v>
+        <v>0.8041894500608463</v>
+      </c>
+      <c r="F11">
+        <v>0.6315695168996384</v>
       </c>
       <c r="H11">
-        <v>-0.1506489769386493</v>
+        <v>0.6010659765620737</v>
       </c>
       <c r="I11">
-        <v>0.6522674128189277</v>
+        <v>0.445985760966529</v>
       </c>
       <c r="J11">
+        <v>0.1987560697275382</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
         <v>0.2525430715716202</v>
       </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>0.1177035147288679</v>
-      </c>
       <c r="M11">
-        <v>0.9363545332786369</v>
+        <v>-0.1349869902559086</v>
       </c>
       <c r="N11">
-        <v>-0.07480865452710381</v>
+        <v>0.05601955201777537</v>
       </c>
       <c r="O11">
-        <v>0.7459856900792554</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+        <v>0.5188514403663723</v>
+      </c>
+      <c r="P11">
+        <v>0.1893413854013475</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-0.07828834604569371</v>
+        <v>0.07053265861265146</v>
       </c>
       <c r="C12">
-        <v>0.04876962339280161</v>
+        <v>-0.02914244125909981</v>
       </c>
       <c r="D12">
-        <v>-0.01463024890903251</v>
+        <v>-0.142443795964709</v>
       </c>
       <c r="E12">
-        <v>-0.09781173102871583</v>
-      </c>
-      <c r="G12">
-        <v>-0.0427452430127298</v>
+        <v>0.1418704476126033</v>
+      </c>
+      <c r="F12">
+        <v>0.06432798670309411</v>
       </c>
       <c r="H12">
-        <v>-0.3230280538554612</v>
+        <v>0.1802842195832685</v>
       </c>
       <c r="I12">
-        <v>0.114092003527871</v>
+        <v>-0.1506489769386493</v>
       </c>
       <c r="J12">
-        <v>-0.1349869902559086</v>
+        <v>0.6522674128189277</v>
       </c>
       <c r="K12">
+        <v>0.2525430715716202</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
         <v>0.1177035147288679</v>
       </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>0.1285181598510687</v>
-      </c>
       <c r="N12">
-        <v>-0.2839976291441505</v>
+        <v>0.9363545332786369</v>
       </c>
       <c r="O12">
-        <v>-0.02349543624334667</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
+        <v>-0.07480865452710381</v>
+      </c>
+      <c r="P12">
+        <v>0.7459856900792554</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.004732017893733165</v>
+        <v>-0.07450578906792989</v>
       </c>
       <c r="C13">
-        <v>0.01742559811962423</v>
+        <v>0.04876962339280161</v>
       </c>
       <c r="D13">
-        <v>0.05679644052597838</v>
+        <v>0.1077856607014213</v>
       </c>
       <c r="E13">
-        <v>-0.1980138146036305</v>
-      </c>
-      <c r="G13">
-        <v>-0.07627511032712242</v>
+        <v>-0.01463024890903251</v>
+      </c>
+      <c r="F13">
+        <v>-0.09781173102871583</v>
       </c>
       <c r="H13">
-        <v>-0.225486848726541</v>
+        <v>-0.0427452430127298</v>
       </c>
       <c r="I13">
-        <v>0.4944986209532007</v>
+        <v>-0.3230280538554612</v>
       </c>
       <c r="J13">
-        <v>0.05601955201777537</v>
+        <v>0.114092003527871</v>
       </c>
       <c r="K13">
-        <v>0.9363545332786369</v>
+        <v>-0.1349869902559086</v>
       </c>
       <c r="L13">
+        <v>0.1177035147288679</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
         <v>0.1285181598510687</v>
       </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <v>-0.1775736450325868</v>
-      </c>
       <c r="O13">
-        <v>0.6916111360249111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+        <v>-0.2839976291441505</v>
+      </c>
+      <c r="P13">
+        <v>-0.02349543624334667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-0.08118141911519945</v>
+        <v>0.03265917347778867</v>
       </c>
       <c r="C14">
-        <v>0.06934592894886464</v>
+        <v>0.01742559811962423</v>
       </c>
       <c r="D14">
-        <v>0.3661331865400339</v>
+        <v>-0.06144998064813029</v>
       </c>
       <c r="E14">
-        <v>0.4101233346279459</v>
-      </c>
-      <c r="G14">
-        <v>0.3858841094161588</v>
+        <v>0.05679644052597838</v>
+      </c>
+      <c r="F14">
+        <v>-0.1980138146036305</v>
       </c>
       <c r="H14">
-        <v>0.9082083413765707</v>
+        <v>-0.07627511032712242</v>
       </c>
       <c r="I14">
-        <v>-0.1579486423221279</v>
+        <v>-0.225486848726541</v>
       </c>
       <c r="J14">
-        <v>0.5188514403663723</v>
+        <v>0.4944986209532007</v>
       </c>
       <c r="K14">
-        <v>-0.07480865452710381</v>
+        <v>0.05601955201777537</v>
       </c>
       <c r="L14">
-        <v>-0.2839976291441505</v>
+        <v>0.9363545332786369</v>
       </c>
       <c r="M14">
+        <v>0.1285181598510687</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
         <v>-0.1775736450325868</v>
       </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-      <c r="O14">
-        <v>-0.1765699855808679</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="P14">
+        <v>0.6916111360249111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-0.02673676715644199</v>
+        <v>0.05382833303964853</v>
       </c>
       <c r="C15">
+        <v>0.06934592894886464</v>
+      </c>
+      <c r="D15">
+        <v>0.1362113189276979</v>
+      </c>
+      <c r="E15">
+        <v>0.3661331865400339</v>
+      </c>
+      <c r="F15">
+        <v>0.4101233346279459</v>
+      </c>
+      <c r="H15">
+        <v>0.3858841094161588</v>
+      </c>
+      <c r="I15">
+        <v>0.9082083413765707</v>
+      </c>
+      <c r="J15">
+        <v>-0.1579486423221279</v>
+      </c>
+      <c r="K15">
+        <v>0.5188514403663723</v>
+      </c>
+      <c r="L15">
+        <v>-0.07480865452710381</v>
+      </c>
+      <c r="M15">
+        <v>-0.2839976291441505</v>
+      </c>
+      <c r="N15">
+        <v>-0.1775736450325868</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>-0.1765699855808679</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>-0.009843459895422251</v>
+      </c>
+      <c r="C16">
         <v>0.06306186227928907</v>
       </c>
-      <c r="D15">
+      <c r="D16">
+        <v>-0.1364125383050702</v>
+      </c>
+      <c r="E16">
         <v>0.04245051279411372</v>
       </c>
-      <c r="E15">
+      <c r="F16">
         <v>0.09082176799679093</v>
       </c>
-      <c r="G15">
+      <c r="H16">
         <v>0.1521262490988143</v>
       </c>
-      <c r="H15">
+      <c r="I16">
         <v>-0.1723749541018063</v>
       </c>
-      <c r="I15">
+      <c r="J16">
         <v>0.7403132706269152</v>
       </c>
-      <c r="J15">
+      <c r="K16">
         <v>0.1893413854013475</v>
       </c>
-      <c r="K15">
+      <c r="L16">
         <v>0.7459856900792554</v>
       </c>
-      <c r="L15">
+      <c r="M16">
         <v>-0.02349543624334667</v>
       </c>
-      <c r="M15">
+      <c r="N16">
         <v>0.6916111360249111</v>
       </c>
-      <c r="N15">
+      <c r="O16">
         <v>-0.1765699855808679</v>
       </c>
-      <c r="O15">
+      <c r="P16">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
time series plot show wage growth negatively correlated average perceived risk.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corrM.xlsx
+++ b/WorkingFolder/Tables/corrM.xlsx
@@ -477,43 +477,43 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>-0.4739381494412931</v>
+        <v>-0.7047556261015829</v>
       </c>
       <c r="D2">
-        <v>0.01919449350673576</v>
+        <v>-0.1005524227762842</v>
       </c>
       <c r="E2">
-        <v>0.1353018484758965</v>
+        <v>-0.04743437747629582</v>
       </c>
       <c r="F2">
-        <v>0.09068930835106143</v>
+        <v>0.02275530254629318</v>
       </c>
       <c r="H2">
-        <v>0.03676615276217467</v>
+        <v>0.01984950350403698</v>
       </c>
       <c r="I2">
-        <v>0.1295600575368288</v>
+        <v>-0.07735816559944704</v>
       </c>
       <c r="J2">
-        <v>-0.0639152332538617</v>
+        <v>-0.1403061574535686</v>
       </c>
       <c r="K2">
-        <v>0.05640457747579858</v>
+        <v>-0.04671663250852448</v>
       </c>
       <c r="L2">
-        <v>0.07053265861265146</v>
+        <v>0.02676678503401862</v>
       </c>
       <c r="M2">
-        <v>-0.07450578906792989</v>
+        <v>-0.07828834604569371</v>
       </c>
       <c r="N2">
-        <v>0.03265917347778867</v>
+        <v>0.004732017893733165</v>
       </c>
       <c r="O2">
-        <v>0.05382833303964853</v>
+        <v>-0.08118141911519945</v>
       </c>
       <c r="P2">
-        <v>-0.009843459895422251</v>
+        <v>-0.02673676715644199</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -521,13 +521,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-0.4739381494412931</v>
+        <v>-0.7047556261015829</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.1023066948649261</v>
+        <v>0.140323046109499</v>
       </c>
       <c r="E3">
         <v>0.07440478395551647</v>
@@ -568,46 +568,46 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.01919449350673576</v>
+        <v>-0.1005524227762842</v>
       </c>
       <c r="C4">
-        <v>0.1023066948649261</v>
+        <v>0.140323046109499</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.0664357926112886</v>
+        <v>0.2912621032440872</v>
       </c>
       <c r="F4">
-        <v>-0.1564425234255272</v>
+        <v>-0.1478776120475858</v>
       </c>
       <c r="H4">
-        <v>-0.2202972830706263</v>
+        <v>-0.1909117508911267</v>
       </c>
       <c r="I4">
-        <v>0.1483430455084005</v>
+        <v>0.3510319043220564</v>
       </c>
       <c r="J4">
-        <v>-0.2082208012276153</v>
+        <v>-0.4814546273730555</v>
       </c>
       <c r="K4">
-        <v>-0.02102817223964968</v>
+        <v>0.03448084153235571</v>
       </c>
       <c r="L4">
-        <v>-0.142443795964709</v>
+        <v>-0.3926606960539389</v>
       </c>
       <c r="M4">
-        <v>0.1077856607014213</v>
+        <v>0.0682481025881473</v>
       </c>
       <c r="N4">
-        <v>-0.06144998064813029</v>
+        <v>-0.2865747988606426</v>
       </c>
       <c r="O4">
-        <v>0.1362113189276979</v>
+        <v>0.2750477972531822</v>
       </c>
       <c r="P4">
-        <v>-0.1364125383050702</v>
+        <v>-0.4368722050314565</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -615,13 +615,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.1353018484758965</v>
+        <v>-0.04743437747629582</v>
       </c>
       <c r="C5">
         <v>0.07440478395551647</v>
       </c>
       <c r="D5">
-        <v>0.0664357926112886</v>
+        <v>0.2912621032440872</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -662,13 +662,13 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.09068930835106143</v>
+        <v>0.02275530254629318</v>
       </c>
       <c r="C6">
         <v>-0.06986646035450562</v>
       </c>
       <c r="D6">
-        <v>-0.1564425234255272</v>
+        <v>-0.1478776120475858</v>
       </c>
       <c r="E6">
         <v>0.3456618958283406</v>
@@ -714,13 +714,13 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.03676615276217467</v>
+        <v>0.01984950350403698</v>
       </c>
       <c r="C8">
         <v>-0.06051795811232875</v>
       </c>
       <c r="D8">
-        <v>-0.2202972830706263</v>
+        <v>-0.1909117508911267</v>
       </c>
       <c r="E8">
         <v>0.3269328383725711</v>
@@ -761,13 +761,13 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.1295600575368288</v>
+        <v>-0.07735816559944704</v>
       </c>
       <c r="C9">
         <v>0.1143498427673656</v>
       </c>
       <c r="D9">
-        <v>0.1483430455084005</v>
+        <v>0.3510319043220564</v>
       </c>
       <c r="E9">
         <v>0.3958692142618715</v>
@@ -808,13 +808,13 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-0.0639152332538617</v>
+        <v>-0.1403061574535686</v>
       </c>
       <c r="C10">
         <v>0.09527665589281313</v>
       </c>
       <c r="D10">
-        <v>-0.2082208012276153</v>
+        <v>-0.4814546273730555</v>
       </c>
       <c r="E10">
         <v>0.03844707986648056</v>
@@ -855,13 +855,13 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.05640457747579858</v>
+        <v>-0.04671663250852448</v>
       </c>
       <c r="C11">
         <v>-0.01151755191354742</v>
       </c>
       <c r="D11">
-        <v>-0.02102817223964968</v>
+        <v>0.03448084153235571</v>
       </c>
       <c r="E11">
         <v>0.8041894500608463</v>
@@ -902,13 +902,13 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.07053265861265146</v>
+        <v>0.02676678503401862</v>
       </c>
       <c r="C12">
         <v>-0.02914244125909981</v>
       </c>
       <c r="D12">
-        <v>-0.142443795964709</v>
+        <v>-0.3926606960539389</v>
       </c>
       <c r="E12">
         <v>0.1418704476126033</v>
@@ -949,13 +949,13 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-0.07450578906792989</v>
+        <v>-0.07828834604569371</v>
       </c>
       <c r="C13">
         <v>0.04876962339280161</v>
       </c>
       <c r="D13">
-        <v>0.1077856607014213</v>
+        <v>0.0682481025881473</v>
       </c>
       <c r="E13">
         <v>-0.01463024890903251</v>
@@ -996,13 +996,13 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.03265917347778867</v>
+        <v>0.004732017893733165</v>
       </c>
       <c r="C14">
         <v>0.01742559811962423</v>
       </c>
       <c r="D14">
-        <v>-0.06144998064813029</v>
+        <v>-0.2865747988606426</v>
       </c>
       <c r="E14">
         <v>0.05679644052597838</v>
@@ -1043,13 +1043,13 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.05382833303964853</v>
+        <v>-0.08118141911519945</v>
       </c>
       <c r="C15">
         <v>0.06934592894886464</v>
       </c>
       <c r="D15">
-        <v>0.1362113189276979</v>
+        <v>0.2750477972531822</v>
       </c>
       <c r="E15">
         <v>0.3661331865400339</v>
@@ -1090,13 +1090,13 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-0.009843459895422251</v>
+        <v>-0.02673676715644199</v>
       </c>
       <c r="C16">
         <v>0.06306186227928907</v>
       </c>
       <c r="D16">
-        <v>-0.1364125383050702</v>
+        <v>-0.4368722050314565</v>
       </c>
       <c r="E16">
         <v>0.04245051279411372</v>

</xml_diff>

<commit_message>
more organized regression tables.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corrM.xlsx
+++ b/WorkingFolder/Tables/corrM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>sp500</t>
   </si>
@@ -31,9 +31,6 @@
     <t>iqrMed</t>
   </si>
   <si>
-    <t>skewMed</t>
-  </si>
-  <si>
     <t>varMed</t>
   </si>
   <si>
@@ -47,9 +44,6 @@
   </si>
   <si>
     <t>iqrMean</t>
-  </si>
-  <si>
-    <t>skewMean</t>
   </si>
   <si>
     <t>varMean</t>
@@ -416,13 +410,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,14 +456,8 @@
       <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,35 +476,32 @@
       <c r="F2">
         <v>0.02275530254629318</v>
       </c>
+      <c r="G2">
+        <v>0.01984950350403698</v>
+      </c>
       <c r="H2">
-        <v>0.01984950350403698</v>
+        <v>-0.07735816559944704</v>
       </c>
       <c r="I2">
-        <v>-0.07735816559944704</v>
+        <v>-0.1403061574535686</v>
       </c>
       <c r="J2">
-        <v>-0.1403061574535686</v>
+        <v>-0.04671663250852448</v>
       </c>
       <c r="K2">
-        <v>-0.04671663250852448</v>
+        <v>0.02676678503401862</v>
       </c>
       <c r="L2">
-        <v>0.02676678503401862</v>
+        <v>0.004732017893733165</v>
       </c>
       <c r="M2">
-        <v>-0.07828834604569371</v>
+        <v>-0.08118141911519945</v>
       </c>
       <c r="N2">
-        <v>0.004732017893733165</v>
-      </c>
-      <c r="O2">
-        <v>-0.08118141911519945</v>
-      </c>
-      <c r="P2">
         <v>-0.02673676715644199</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -535,35 +520,32 @@
       <c r="F3">
         <v>-0.06986646035450562</v>
       </c>
+      <c r="G3">
+        <v>-0.06051795811232875</v>
+      </c>
       <c r="H3">
-        <v>-0.06051795811232875</v>
+        <v>0.1143498427673656</v>
       </c>
       <c r="I3">
-        <v>0.1143498427673656</v>
+        <v>0.09527665589281313</v>
       </c>
       <c r="J3">
-        <v>0.09527665589281313</v>
+        <v>-0.01151755191354742</v>
       </c>
       <c r="K3">
-        <v>-0.01151755191354742</v>
+        <v>-0.02914244125909981</v>
       </c>
       <c r="L3">
-        <v>-0.02914244125909981</v>
+        <v>0.01742559811962423</v>
       </c>
       <c r="M3">
-        <v>0.04876962339280161</v>
+        <v>0.06934592894886464</v>
       </c>
       <c r="N3">
-        <v>0.01742559811962423</v>
-      </c>
-      <c r="O3">
-        <v>0.06934592894886464</v>
-      </c>
-      <c r="P3">
         <v>0.06306186227928907</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -582,35 +564,32 @@
       <c r="F4">
         <v>-0.1478776120475858</v>
       </c>
+      <c r="G4">
+        <v>-0.1909117508911267</v>
+      </c>
       <c r="H4">
-        <v>-0.1909117508911267</v>
+        <v>0.3510319043220564</v>
       </c>
       <c r="I4">
-        <v>0.3510319043220564</v>
+        <v>-0.4814546273730555</v>
       </c>
       <c r="J4">
-        <v>-0.4814546273730555</v>
+        <v>0.03448084153235571</v>
       </c>
       <c r="K4">
-        <v>0.03448084153235571</v>
+        <v>-0.3926606960539389</v>
       </c>
       <c r="L4">
-        <v>-0.3926606960539389</v>
+        <v>-0.2865747988606426</v>
       </c>
       <c r="M4">
-        <v>0.0682481025881473</v>
+        <v>0.2750477972531822</v>
       </c>
       <c r="N4">
-        <v>-0.2865747988606426</v>
-      </c>
-      <c r="O4">
-        <v>0.2750477972531822</v>
-      </c>
-      <c r="P4">
         <v>-0.4368722050314565</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -629,35 +608,32 @@
       <c r="F5">
         <v>0.3456618958283406</v>
       </c>
+      <c r="G5">
+        <v>0.3269328383725711</v>
+      </c>
       <c r="H5">
-        <v>0.3269328383725711</v>
+        <v>0.3958692142618715</v>
       </c>
       <c r="I5">
-        <v>0.3958692142618715</v>
+        <v>0.03844707986648056</v>
       </c>
       <c r="J5">
-        <v>0.03844707986648056</v>
+        <v>0.8041894500608463</v>
       </c>
       <c r="K5">
-        <v>0.8041894500608463</v>
+        <v>0.1418704476126033</v>
       </c>
       <c r="L5">
-        <v>0.1418704476126033</v>
+        <v>0.05679644052597838</v>
       </c>
       <c r="M5">
-        <v>-0.01463024890903251</v>
+        <v>0.3661331865400339</v>
       </c>
       <c r="N5">
-        <v>0.05679644052597838</v>
-      </c>
-      <c r="O5">
-        <v>0.3661331865400339</v>
-      </c>
-      <c r="P5">
         <v>0.04245051279411372</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -676,459 +652,380 @@
       <c r="F6">
         <v>1</v>
       </c>
+      <c r="G6">
+        <v>0.952956949937701</v>
+      </c>
       <c r="H6">
-        <v>0.952956949937701</v>
+        <v>0.3616315137833193</v>
       </c>
       <c r="I6">
-        <v>0.3616315137833193</v>
+        <v>0.3244402953268535</v>
       </c>
       <c r="J6">
-        <v>0.3244402953268535</v>
+        <v>0.6315695168996384</v>
       </c>
       <c r="K6">
-        <v>0.6315695168996384</v>
+        <v>0.06432798670309411</v>
       </c>
       <c r="L6">
-        <v>0.06432798670309411</v>
+        <v>-0.1980138146036305</v>
       </c>
       <c r="M6">
-        <v>-0.09781173102871583</v>
+        <v>0.4101233346279459</v>
       </c>
       <c r="N6">
-        <v>-0.1980138146036305</v>
-      </c>
-      <c r="O6">
-        <v>0.4101233346279459</v>
-      </c>
-      <c r="P6">
         <v>0.09082176799679093</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="B7">
+        <v>0.01984950350403698</v>
+      </c>
+      <c r="C7">
+        <v>-0.06051795811232875</v>
+      </c>
+      <c r="D7">
+        <v>-0.1909117508911267</v>
+      </c>
+      <c r="E7">
+        <v>0.3269328383725711</v>
+      </c>
+      <c r="F7">
+        <v>0.952956949937701</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0.3122748691730542</v>
+      </c>
+      <c r="I7">
+        <v>0.3819806403851467</v>
+      </c>
+      <c r="J7">
+        <v>0.6010659765620737</v>
+      </c>
+      <c r="K7">
+        <v>0.1802842195832685</v>
+      </c>
+      <c r="L7">
+        <v>-0.07627511032712242</v>
+      </c>
+      <c r="M7">
+        <v>0.3858841094161588</v>
+      </c>
+      <c r="N7">
+        <v>0.1521262490988143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.01984950350403698</v>
+        <v>-0.07735816559944704</v>
       </c>
       <c r="C8">
-        <v>-0.06051795811232875</v>
+        <v>0.1143498427673656</v>
       </c>
       <c r="D8">
-        <v>-0.1909117508911267</v>
+        <v>0.3510319043220564</v>
       </c>
       <c r="E8">
-        <v>0.3269328383725711</v>
+        <v>0.3958692142618715</v>
       </c>
       <c r="F8">
-        <v>0.952956949937701</v>
+        <v>0.3616315137833193</v>
+      </c>
+      <c r="G8">
+        <v>0.3122748691730542</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>0.3122748691730542</v>
+        <v>-0.2083907738613129</v>
       </c>
       <c r="J8">
-        <v>0.3819806403851467</v>
+        <v>0.445985760966529</v>
       </c>
       <c r="K8">
-        <v>0.6010659765620737</v>
+        <v>-0.1506489769386493</v>
       </c>
       <c r="L8">
-        <v>0.1802842195832685</v>
+        <v>-0.225486848726541</v>
       </c>
       <c r="M8">
-        <v>-0.0427452430127298</v>
+        <v>0.9082083413765707</v>
       </c>
       <c r="N8">
-        <v>-0.07627511032712242</v>
-      </c>
-      <c r="O8">
-        <v>0.3858841094161588</v>
-      </c>
-      <c r="P8">
-        <v>0.1521262490988143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+        <v>-0.1723749541018063</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-0.07735816559944704</v>
+        <v>-0.1403061574535686</v>
       </c>
       <c r="C9">
-        <v>0.1143498427673656</v>
+        <v>0.09527665589281313</v>
       </c>
       <c r="D9">
-        <v>0.3510319043220564</v>
+        <v>-0.4814546273730555</v>
       </c>
       <c r="E9">
-        <v>0.3958692142618715</v>
+        <v>0.03844707986648056</v>
       </c>
       <c r="F9">
-        <v>0.3616315137833193</v>
+        <v>0.3244402953268535</v>
+      </c>
+      <c r="G9">
+        <v>0.3819806403851467</v>
       </c>
       <c r="H9">
-        <v>0.3122748691730542</v>
+        <v>-0.2083907738613129</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>-0.2083907738613129</v>
+        <v>0.1987560697275382</v>
       </c>
       <c r="K9">
-        <v>0.445985760966529</v>
+        <v>0.6522674128189277</v>
       </c>
       <c r="L9">
-        <v>-0.1506489769386493</v>
+        <v>0.4944986209532007</v>
       </c>
       <c r="M9">
-        <v>-0.3230280538554612</v>
+        <v>-0.1579486423221279</v>
       </c>
       <c r="N9">
-        <v>-0.225486848726541</v>
-      </c>
-      <c r="O9">
-        <v>0.9082083413765707</v>
-      </c>
-      <c r="P9">
-        <v>-0.1723749541018063</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+        <v>0.7403132706269152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-0.1403061574535686</v>
+        <v>-0.04671663250852448</v>
       </c>
       <c r="C10">
-        <v>0.09527665589281313</v>
+        <v>-0.01151755191354742</v>
       </c>
       <c r="D10">
-        <v>-0.4814546273730555</v>
+        <v>0.03448084153235571</v>
       </c>
       <c r="E10">
-        <v>0.03844707986648056</v>
+        <v>0.8041894500608463</v>
       </c>
       <c r="F10">
-        <v>0.3244402953268535</v>
+        <v>0.6315695168996384</v>
+      </c>
+      <c r="G10">
+        <v>0.6010659765620737</v>
       </c>
       <c r="H10">
-        <v>0.3819806403851467</v>
+        <v>0.445985760966529</v>
       </c>
       <c r="I10">
-        <v>-0.2083907738613129</v>
+        <v>0.1987560697275382</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0.1987560697275382</v>
+        <v>0.2525430715716202</v>
       </c>
       <c r="L10">
-        <v>0.6522674128189277</v>
+        <v>0.05601955201777537</v>
       </c>
       <c r="M10">
-        <v>0.114092003527871</v>
+        <v>0.5188514403663723</v>
       </c>
       <c r="N10">
-        <v>0.4944986209532007</v>
-      </c>
-      <c r="O10">
-        <v>-0.1579486423221279</v>
-      </c>
-      <c r="P10">
-        <v>0.7403132706269152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+        <v>0.1893413854013475</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-0.04671663250852448</v>
+        <v>0.02676678503401862</v>
       </c>
       <c r="C11">
-        <v>-0.01151755191354742</v>
+        <v>-0.02914244125909981</v>
       </c>
       <c r="D11">
-        <v>0.03448084153235571</v>
+        <v>-0.3926606960539389</v>
       </c>
       <c r="E11">
-        <v>0.8041894500608463</v>
+        <v>0.1418704476126033</v>
       </c>
       <c r="F11">
-        <v>0.6315695168996384</v>
+        <v>0.06432798670309411</v>
+      </c>
+      <c r="G11">
+        <v>0.1802842195832685</v>
       </c>
       <c r="H11">
-        <v>0.6010659765620737</v>
+        <v>-0.1506489769386493</v>
       </c>
       <c r="I11">
-        <v>0.445985760966529</v>
+        <v>0.6522674128189277</v>
       </c>
       <c r="J11">
-        <v>0.1987560697275382</v>
+        <v>0.2525430715716202</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0.2525430715716202</v>
+        <v>0.9363545332786369</v>
       </c>
       <c r="M11">
-        <v>-0.1349869902559086</v>
+        <v>-0.07480865452710381</v>
       </c>
       <c r="N11">
-        <v>0.05601955201777537</v>
-      </c>
-      <c r="O11">
-        <v>0.5188514403663723</v>
-      </c>
-      <c r="P11">
-        <v>0.1893413854013475</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+        <v>0.7459856900792554</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.02676678503401862</v>
+        <v>0.004732017893733165</v>
       </c>
       <c r="C12">
-        <v>-0.02914244125909981</v>
+        <v>0.01742559811962423</v>
       </c>
       <c r="D12">
-        <v>-0.3926606960539389</v>
+        <v>-0.2865747988606426</v>
       </c>
       <c r="E12">
-        <v>0.1418704476126033</v>
+        <v>0.05679644052597838</v>
       </c>
       <c r="F12">
-        <v>0.06432798670309411</v>
+        <v>-0.1980138146036305</v>
+      </c>
+      <c r="G12">
+        <v>-0.07627511032712242</v>
       </c>
       <c r="H12">
-        <v>0.1802842195832685</v>
+        <v>-0.225486848726541</v>
       </c>
       <c r="I12">
-        <v>-0.1506489769386493</v>
+        <v>0.4944986209532007</v>
       </c>
       <c r="J12">
-        <v>0.6522674128189277</v>
+        <v>0.05601955201777537</v>
       </c>
       <c r="K12">
-        <v>0.2525430715716202</v>
+        <v>0.9363545332786369</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>0.1177035147288679</v>
+        <v>-0.1775736450325868</v>
       </c>
       <c r="N12">
-        <v>0.9363545332786369</v>
-      </c>
-      <c r="O12">
-        <v>-0.07480865452710381</v>
-      </c>
-      <c r="P12">
-        <v>0.7459856900792554</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
+        <v>0.6916111360249111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-0.07828834604569371</v>
+        <v>-0.08118141911519945</v>
       </c>
       <c r="C13">
-        <v>0.04876962339280161</v>
+        <v>0.06934592894886464</v>
       </c>
       <c r="D13">
-        <v>0.0682481025881473</v>
+        <v>0.2750477972531822</v>
       </c>
       <c r="E13">
-        <v>-0.01463024890903251</v>
+        <v>0.3661331865400339</v>
       </c>
       <c r="F13">
-        <v>-0.09781173102871583</v>
+        <v>0.4101233346279459</v>
+      </c>
+      <c r="G13">
+        <v>0.3858841094161588</v>
       </c>
       <c r="H13">
-        <v>-0.0427452430127298</v>
+        <v>0.9082083413765707</v>
       </c>
       <c r="I13">
-        <v>-0.3230280538554612</v>
+        <v>-0.1579486423221279</v>
       </c>
       <c r="J13">
-        <v>0.114092003527871</v>
+        <v>0.5188514403663723</v>
       </c>
       <c r="K13">
-        <v>-0.1349869902559086</v>
+        <v>-0.07480865452710381</v>
       </c>
       <c r="L13">
-        <v>0.1177035147288679</v>
+        <v>-0.1775736450325868</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>0.1285181598510687</v>
-      </c>
-      <c r="O13">
-        <v>-0.2839976291441505</v>
-      </c>
-      <c r="P13">
-        <v>-0.02349543624334667</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>-0.1765699855808679</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.004732017893733165</v>
+        <v>-0.02673676715644199</v>
       </c>
       <c r="C14">
-        <v>0.01742559811962423</v>
+        <v>0.06306186227928907</v>
       </c>
       <c r="D14">
-        <v>-0.2865747988606426</v>
+        <v>-0.4368722050314565</v>
       </c>
       <c r="E14">
-        <v>0.05679644052597838</v>
+        <v>0.04245051279411372</v>
       </c>
       <c r="F14">
-        <v>-0.1980138146036305</v>
+        <v>0.09082176799679093</v>
+      </c>
+      <c r="G14">
+        <v>0.1521262490988143</v>
       </c>
       <c r="H14">
-        <v>-0.07627511032712242</v>
+        <v>-0.1723749541018063</v>
       </c>
       <c r="I14">
-        <v>-0.225486848726541</v>
+        <v>0.7403132706269152</v>
       </c>
       <c r="J14">
-        <v>0.4944986209532007</v>
+        <v>0.1893413854013475</v>
       </c>
       <c r="K14">
-        <v>0.05601955201777537</v>
+        <v>0.7459856900792554</v>
       </c>
       <c r="L14">
-        <v>0.9363545332786369</v>
+        <v>0.6916111360249111</v>
       </c>
       <c r="M14">
-        <v>0.1285181598510687</v>
+        <v>-0.1765699855808679</v>
       </c>
       <c r="N14">
-        <v>1</v>
-      </c>
-      <c r="O14">
-        <v>-0.1775736450325868</v>
-      </c>
-      <c r="P14">
-        <v>0.6916111360249111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>-0.08118141911519945</v>
-      </c>
-      <c r="C15">
-        <v>0.06934592894886464</v>
-      </c>
-      <c r="D15">
-        <v>0.2750477972531822</v>
-      </c>
-      <c r="E15">
-        <v>0.3661331865400339</v>
-      </c>
-      <c r="F15">
-        <v>0.4101233346279459</v>
-      </c>
-      <c r="H15">
-        <v>0.3858841094161588</v>
-      </c>
-      <c r="I15">
-        <v>0.9082083413765707</v>
-      </c>
-      <c r="J15">
-        <v>-0.1579486423221279</v>
-      </c>
-      <c r="K15">
-        <v>0.5188514403663723</v>
-      </c>
-      <c r="L15">
-        <v>-0.07480865452710381</v>
-      </c>
-      <c r="M15">
-        <v>-0.2839976291441505</v>
-      </c>
-      <c r="N15">
-        <v>-0.1775736450325868</v>
-      </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="P15">
-        <v>-0.1765699855808679</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>-0.02673676715644199</v>
-      </c>
-      <c r="C16">
-        <v>0.06306186227928907</v>
-      </c>
-      <c r="D16">
-        <v>-0.4368722050314565</v>
-      </c>
-      <c r="E16">
-        <v>0.04245051279411372</v>
-      </c>
-      <c r="F16">
-        <v>0.09082176799679093</v>
-      </c>
-      <c r="H16">
-        <v>0.1521262490988143</v>
-      </c>
-      <c r="I16">
-        <v>-0.1723749541018063</v>
-      </c>
-      <c r="J16">
-        <v>0.7403132706269152</v>
-      </c>
-      <c r="K16">
-        <v>0.1893413854013475</v>
-      </c>
-      <c r="L16">
-        <v>0.7459856900792554</v>
-      </c>
-      <c r="M16">
-        <v>-0.02349543624334667</v>
-      </c>
-      <c r="N16">
-        <v>0.6916111360249111</v>
-      </c>
-      <c r="O16">
-        <v>-0.1765699855808679</v>
-      </c>
-      <c r="P16">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated data and results till 2020 Jan.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corrM.xlsx
+++ b/WorkingFolder/Tables/corrM.xlsx
@@ -465,40 +465,40 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>-0.7047556261015829</v>
+        <v>-0.680182012841634</v>
       </c>
       <c r="D2">
-        <v>-0.1005524227762842</v>
+        <v>-0.0783303930584449</v>
       </c>
       <c r="E2">
-        <v>-0.04743437747629582</v>
+        <v>-0.03052985330403633</v>
       </c>
       <c r="F2">
-        <v>0.02275530254629318</v>
+        <v>0.01371389403032016</v>
       </c>
       <c r="G2">
-        <v>0.01984950350403698</v>
+        <v>0.0124000437774399</v>
       </c>
       <c r="H2">
-        <v>-0.07735816559944704</v>
+        <v>-0.04819288080125357</v>
       </c>
       <c r="I2">
-        <v>-0.1403061574535686</v>
+        <v>-0.1023235157253121</v>
       </c>
       <c r="J2">
-        <v>-0.04671663250852448</v>
+        <v>-0.01461638364964552</v>
       </c>
       <c r="K2">
-        <v>0.02676678503401862</v>
+        <v>0.05652648764826258</v>
       </c>
       <c r="L2">
-        <v>0.004732017893733165</v>
+        <v>0.02823333018647582</v>
       </c>
       <c r="M2">
-        <v>-0.08118141911519945</v>
+        <v>-0.03196208928288601</v>
       </c>
       <c r="N2">
-        <v>-0.02673676715644199</v>
+        <v>-0.01748914489945714</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -506,43 +506,43 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-0.7047556261015829</v>
+        <v>-0.680182012841634</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.140323046109499</v>
+        <v>0.1221720518472285</v>
       </c>
       <c r="E3">
-        <v>0.07440478395551647</v>
+        <v>0.05653006462466296</v>
       </c>
       <c r="F3">
-        <v>-0.06986646035450562</v>
+        <v>-0.05391471495687534</v>
       </c>
       <c r="G3">
-        <v>-0.06051795811232875</v>
+        <v>-0.06253280915464397</v>
       </c>
       <c r="H3">
-        <v>0.1143498427673656</v>
+        <v>0.1111497886989482</v>
       </c>
       <c r="I3">
-        <v>0.09527665589281313</v>
+        <v>0.06909878822468789</v>
       </c>
       <c r="J3">
-        <v>-0.01151755191354742</v>
+        <v>-0.01909015669427782</v>
       </c>
       <c r="K3">
-        <v>-0.02914244125909981</v>
+        <v>-0.04374136016896989</v>
       </c>
       <c r="L3">
-        <v>0.01742559811962423</v>
+        <v>0.006575284563791996</v>
       </c>
       <c r="M3">
-        <v>0.06934592894886464</v>
+        <v>0.07679382384287423</v>
       </c>
       <c r="N3">
-        <v>0.06306186227928907</v>
+        <v>0.03795934618164015</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -550,43 +550,43 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.1005524227762842</v>
+        <v>-0.0783303930584449</v>
       </c>
       <c r="C4">
-        <v>0.140323046109499</v>
+        <v>0.1221720518472285</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.2912621032440872</v>
+        <v>0.2981098520604903</v>
       </c>
       <c r="F4">
-        <v>-0.1478776120475858</v>
+        <v>-0.1633195338039325</v>
       </c>
       <c r="G4">
-        <v>-0.1909117508911267</v>
+        <v>-0.1470984054862519</v>
       </c>
       <c r="H4">
-        <v>0.3510319043220564</v>
+        <v>0.3588750911617425</v>
       </c>
       <c r="I4">
-        <v>-0.4814546273730555</v>
+        <v>-0.5151684230962238</v>
       </c>
       <c r="J4">
-        <v>0.03448084153235571</v>
+        <v>0.01043230032222128</v>
       </c>
       <c r="K4">
-        <v>-0.3926606960539389</v>
+        <v>-0.459597172319483</v>
       </c>
       <c r="L4">
-        <v>-0.2865747988606426</v>
+        <v>-0.342156576835674</v>
       </c>
       <c r="M4">
-        <v>0.2750477972531822</v>
+        <v>0.3420214029909316</v>
       </c>
       <c r="N4">
-        <v>-0.4368722050314565</v>
+        <v>-0.4634142680280373</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -594,43 +594,43 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-0.04743437747629582</v>
+        <v>-0.03052985330403633</v>
       </c>
       <c r="C5">
-        <v>0.07440478395551647</v>
+        <v>0.05653006462466296</v>
       </c>
       <c r="D5">
-        <v>0.2912621032440872</v>
+        <v>0.2981098520604903</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.3456618958283406</v>
+        <v>0.3612509639485904</v>
       </c>
       <c r="G5">
-        <v>0.3269328383725711</v>
+        <v>0.3641198327393359</v>
       </c>
       <c r="H5">
-        <v>0.3958692142618715</v>
+        <v>0.4127631093249592</v>
       </c>
       <c r="I5">
-        <v>0.03844707986648056</v>
+        <v>0.03599422413450309</v>
       </c>
       <c r="J5">
-        <v>0.8041894500608463</v>
+        <v>0.7921024341773386</v>
       </c>
       <c r="K5">
-        <v>0.1418704476126033</v>
+        <v>0.08673123342589122</v>
       </c>
       <c r="L5">
-        <v>0.05679644052597838</v>
+        <v>-0.002601885874268448</v>
       </c>
       <c r="M5">
-        <v>0.3661331865400339</v>
+        <v>0.3904627113860717</v>
       </c>
       <c r="N5">
-        <v>0.04245051279411372</v>
+        <v>-0.0004828960342666396</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -638,43 +638,43 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.02275530254629318</v>
+        <v>0.01371389403032016</v>
       </c>
       <c r="C6">
-        <v>-0.06986646035450562</v>
+        <v>-0.05391471495687534</v>
       </c>
       <c r="D6">
-        <v>-0.1478776120475858</v>
+        <v>-0.1633195338039325</v>
       </c>
       <c r="E6">
-        <v>0.3456618958283406</v>
+        <v>0.3612509639485904</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.952956949937701</v>
+        <v>0.9809329076610995</v>
       </c>
       <c r="H6">
-        <v>0.3616315137833193</v>
+        <v>0.3722554629941501</v>
       </c>
       <c r="I6">
-        <v>0.3244402953268535</v>
+        <v>0.1806114662513572</v>
       </c>
       <c r="J6">
-        <v>0.6315695168996384</v>
+        <v>0.6301873021039683</v>
       </c>
       <c r="K6">
-        <v>0.06432798670309411</v>
+        <v>-0.04454127211874876</v>
       </c>
       <c r="L6">
-        <v>-0.1980138146036305</v>
+        <v>-0.3129315469833898</v>
       </c>
       <c r="M6">
-        <v>0.4101233346279459</v>
+        <v>0.3725002900626034</v>
       </c>
       <c r="N6">
-        <v>0.09082176799679093</v>
+        <v>0.05618209907557382</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -682,43 +682,43 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.01984950350403698</v>
+        <v>0.0124000437774399</v>
       </c>
       <c r="C7">
-        <v>-0.06051795811232875</v>
+        <v>-0.06253280915464397</v>
       </c>
       <c r="D7">
-        <v>-0.1909117508911267</v>
+        <v>-0.1470984054862519</v>
       </c>
       <c r="E7">
-        <v>0.3269328383725711</v>
+        <v>0.3641198327393359</v>
       </c>
       <c r="F7">
-        <v>0.952956949937701</v>
+        <v>0.9809329076610995</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.3122748691730542</v>
+        <v>0.3743625636196435</v>
       </c>
       <c r="I7">
-        <v>0.3819806403851467</v>
+        <v>0.2414502345040999</v>
       </c>
       <c r="J7">
-        <v>0.6010659765620737</v>
+        <v>0.6426601479267363</v>
       </c>
       <c r="K7">
-        <v>0.1802842195832685</v>
+        <v>0.008927636603904878</v>
       </c>
       <c r="L7">
-        <v>-0.07627511032712242</v>
+        <v>-0.268192419546511</v>
       </c>
       <c r="M7">
-        <v>0.3858841094161588</v>
+        <v>0.3823050395265182</v>
       </c>
       <c r="N7">
-        <v>0.1521262490988143</v>
+        <v>0.07325264309598917</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -726,43 +726,43 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.07735816559944704</v>
+        <v>-0.04819288080125357</v>
       </c>
       <c r="C8">
-        <v>0.1143498427673656</v>
+        <v>0.1111497886989482</v>
       </c>
       <c r="D8">
-        <v>0.3510319043220564</v>
+        <v>0.3588750911617425</v>
       </c>
       <c r="E8">
-        <v>0.3958692142618715</v>
+        <v>0.4127631093249592</v>
       </c>
       <c r="F8">
-        <v>0.3616315137833193</v>
+        <v>0.3722554629941501</v>
       </c>
       <c r="G8">
-        <v>0.3122748691730542</v>
+        <v>0.3743625636196435</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>-0.2083907738613129</v>
+        <v>-0.1997910261620322</v>
       </c>
       <c r="J8">
-        <v>0.445985760966529</v>
+        <v>0.4475614826426157</v>
       </c>
       <c r="K8">
-        <v>-0.1506489769386493</v>
+        <v>-0.1437392066062044</v>
       </c>
       <c r="L8">
-        <v>-0.225486848726541</v>
+        <v>-0.2180916373139349</v>
       </c>
       <c r="M8">
-        <v>0.9082083413765707</v>
+        <v>0.9172288078615954</v>
       </c>
       <c r="N8">
-        <v>-0.1723749541018063</v>
+        <v>-0.159014452899539</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -770,43 +770,43 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-0.1403061574535686</v>
+        <v>-0.1023235157253121</v>
       </c>
       <c r="C9">
-        <v>0.09527665589281313</v>
+        <v>0.06909878822468789</v>
       </c>
       <c r="D9">
-        <v>-0.4814546273730555</v>
+        <v>-0.5151684230962238</v>
       </c>
       <c r="E9">
-        <v>0.03844707986648056</v>
+        <v>0.03599422413450309</v>
       </c>
       <c r="F9">
-        <v>0.3244402953268535</v>
+        <v>0.1806114662513572</v>
       </c>
       <c r="G9">
-        <v>0.3819806403851467</v>
+        <v>0.2414502345040999</v>
       </c>
       <c r="H9">
-        <v>-0.2083907738613129</v>
+        <v>-0.1997910261620322</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>0.1987560697275382</v>
+        <v>0.2333820891919775</v>
       </c>
       <c r="K9">
-        <v>0.6522674128189277</v>
+        <v>0.6883971392785034</v>
       </c>
       <c r="L9">
-        <v>0.4944986209532007</v>
+        <v>0.5246616647241267</v>
       </c>
       <c r="M9">
-        <v>-0.1579486423221279</v>
+        <v>-0.2193972891311861</v>
       </c>
       <c r="N9">
-        <v>0.7403132706269152</v>
+        <v>0.7480185820308105</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -814,43 +814,43 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-0.04671663250852448</v>
+        <v>-0.01461638364964552</v>
       </c>
       <c r="C10">
-        <v>-0.01151755191354742</v>
+        <v>-0.01909015669427782</v>
       </c>
       <c r="D10">
-        <v>0.03448084153235571</v>
+        <v>0.01043230032222128</v>
       </c>
       <c r="E10">
-        <v>0.8041894500608463</v>
+        <v>0.7921024341773386</v>
       </c>
       <c r="F10">
-        <v>0.6315695168996384</v>
+        <v>0.6301873021039683</v>
       </c>
       <c r="G10">
-        <v>0.6010659765620737</v>
+        <v>0.6426601479267363</v>
       </c>
       <c r="H10">
-        <v>0.445985760966529</v>
+        <v>0.4475614826426157</v>
       </c>
       <c r="I10">
-        <v>0.1987560697275382</v>
+        <v>0.2333820891919775</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0.2525430715716202</v>
+        <v>0.2711736763683567</v>
       </c>
       <c r="L10">
-        <v>0.05601955201777537</v>
+        <v>0.05649703490390926</v>
       </c>
       <c r="M10">
-        <v>0.5188514403663723</v>
+        <v>0.4819490113416408</v>
       </c>
       <c r="N10">
-        <v>0.1893413854013475</v>
+        <v>0.1951778656562174</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -858,43 +858,43 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.02676678503401862</v>
+        <v>0.05652648764826258</v>
       </c>
       <c r="C11">
-        <v>-0.02914244125909981</v>
+        <v>-0.04374136016896989</v>
       </c>
       <c r="D11">
-        <v>-0.3926606960539389</v>
+        <v>-0.459597172319483</v>
       </c>
       <c r="E11">
-        <v>0.1418704476126033</v>
+        <v>0.08673123342589122</v>
       </c>
       <c r="F11">
-        <v>0.06432798670309411</v>
+        <v>-0.04454127211874876</v>
       </c>
       <c r="G11">
-        <v>0.1802842195832685</v>
+        <v>0.008927636603904878</v>
       </c>
       <c r="H11">
-        <v>-0.1506489769386493</v>
+        <v>-0.1437392066062044</v>
       </c>
       <c r="I11">
-        <v>0.6522674128189277</v>
+        <v>0.6883971392785034</v>
       </c>
       <c r="J11">
-        <v>0.2525430715716202</v>
+        <v>0.2711736763683567</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0.9363545332786369</v>
+        <v>0.931601405267243</v>
       </c>
       <c r="M11">
-        <v>-0.07480865452710381</v>
+        <v>-0.13932507739623</v>
       </c>
       <c r="N11">
-        <v>0.7459856900792554</v>
+        <v>0.759344995191208</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -902,43 +902,43 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.004732017893733165</v>
+        <v>0.02823333018647582</v>
       </c>
       <c r="C12">
-        <v>0.01742559811962423</v>
+        <v>0.006575284563791996</v>
       </c>
       <c r="D12">
-        <v>-0.2865747988606426</v>
+        <v>-0.342156576835674</v>
       </c>
       <c r="E12">
-        <v>0.05679644052597838</v>
+        <v>-0.002601885874268448</v>
       </c>
       <c r="F12">
-        <v>-0.1980138146036305</v>
+        <v>-0.3129315469833898</v>
       </c>
       <c r="G12">
-        <v>-0.07627511032712242</v>
+        <v>-0.268192419546511</v>
       </c>
       <c r="H12">
-        <v>-0.225486848726541</v>
+        <v>-0.2180916373139349</v>
       </c>
       <c r="I12">
-        <v>0.4944986209532007</v>
+        <v>0.5246616647241267</v>
       </c>
       <c r="J12">
-        <v>0.05601955201777537</v>
+        <v>0.05649703490390926</v>
       </c>
       <c r="K12">
-        <v>0.9363545332786369</v>
+        <v>0.931601405267243</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>-0.1775736450325868</v>
+        <v>-0.2257734971776478</v>
       </c>
       <c r="N12">
-        <v>0.6916111360249111</v>
+        <v>0.7016434961541568</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -946,43 +946,43 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-0.08118141911519945</v>
+        <v>-0.03196208928288601</v>
       </c>
       <c r="C13">
-        <v>0.06934592894886464</v>
+        <v>0.07679382384287423</v>
       </c>
       <c r="D13">
-        <v>0.2750477972531822</v>
+        <v>0.3420214029909316</v>
       </c>
       <c r="E13">
-        <v>0.3661331865400339</v>
+        <v>0.3904627113860717</v>
       </c>
       <c r="F13">
-        <v>0.4101233346279459</v>
+        <v>0.3725002900626034</v>
       </c>
       <c r="G13">
-        <v>0.3858841094161588</v>
+        <v>0.3823050395265182</v>
       </c>
       <c r="H13">
-        <v>0.9082083413765707</v>
+        <v>0.9172288078615954</v>
       </c>
       <c r="I13">
-        <v>-0.1579486423221279</v>
+        <v>-0.2193972891311861</v>
       </c>
       <c r="J13">
-        <v>0.5188514403663723</v>
+        <v>0.4819490113416408</v>
       </c>
       <c r="K13">
-        <v>-0.07480865452710381</v>
+        <v>-0.13932507739623</v>
       </c>
       <c r="L13">
-        <v>-0.1775736450325868</v>
+        <v>-0.2257734971776478</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>-0.1765699855808679</v>
+        <v>-0.1896858643044187</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -990,40 +990,40 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-0.02673676715644199</v>
+        <v>-0.01748914489945714</v>
       </c>
       <c r="C14">
-        <v>0.06306186227928907</v>
+        <v>0.03795934618164015</v>
       </c>
       <c r="D14">
-        <v>-0.4368722050314565</v>
+        <v>-0.4634142680280373</v>
       </c>
       <c r="E14">
-        <v>0.04245051279411372</v>
+        <v>-0.0004828960342666396</v>
       </c>
       <c r="F14">
-        <v>0.09082176799679093</v>
+        <v>0.05618209907557382</v>
       </c>
       <c r="G14">
-        <v>0.1521262490988143</v>
+        <v>0.07325264309598917</v>
       </c>
       <c r="H14">
-        <v>-0.1723749541018063</v>
+        <v>-0.159014452899539</v>
       </c>
       <c r="I14">
-        <v>0.7403132706269152</v>
+        <v>0.7480185820308105</v>
       </c>
       <c r="J14">
-        <v>0.1893413854013475</v>
+        <v>0.1951778656562174</v>
       </c>
       <c r="K14">
-        <v>0.7459856900792554</v>
+        <v>0.759344995191208</v>
       </c>
       <c r="L14">
-        <v>0.6916111360249111</v>
+        <v>0.7016434961541568</v>
       </c>
       <c r="M14">
-        <v>-0.1765699855808679</v>
+        <v>-0.1896858643044187</v>
       </c>
       <c r="N14">
         <v>1</v>

</xml_diff>

<commit_message>
updated data through Mar2020. solved life-cycle ma model. added small changes to theoretical framework section.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corrM.xlsx
+++ b/WorkingFolder/Tables/corrM.xlsx
@@ -465,40 +465,40 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>-0.680182012841634</v>
+        <v>-0.689801893040383</v>
       </c>
       <c r="D2">
-        <v>-0.0783303930584449</v>
+        <v>-0.1977895957625399</v>
       </c>
       <c r="E2">
-        <v>-0.03052985330403633</v>
+        <v>0.00953015815020954</v>
       </c>
       <c r="F2">
-        <v>0.01371389403032016</v>
+        <v>0.01584236461698259</v>
       </c>
       <c r="G2">
-        <v>0.0124000437774399</v>
+        <v>0.01516645206850985</v>
       </c>
       <c r="H2">
-        <v>-0.04819288080125357</v>
+        <v>-0.05184377338114116</v>
       </c>
       <c r="I2">
-        <v>-0.1023235157253121</v>
+        <v>-0.1409981214786789</v>
       </c>
       <c r="J2">
-        <v>-0.01461638364964552</v>
+        <v>0.03196566811971526</v>
       </c>
       <c r="K2">
-        <v>0.05652648764826258</v>
+        <v>0.0665734164232875</v>
       </c>
       <c r="L2">
-        <v>0.02823333018647582</v>
+        <v>0.04435601442290548</v>
       </c>
       <c r="M2">
-        <v>-0.03196208928288601</v>
+        <v>-0.01419361331937312</v>
       </c>
       <c r="N2">
-        <v>-0.01748914489945714</v>
+        <v>-0.03413895618995193</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -506,43 +506,43 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-0.680182012841634</v>
+        <v>-0.689801893040383</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.1221720518472285</v>
+        <v>0.1754789520186602</v>
       </c>
       <c r="E3">
-        <v>0.05653006462466296</v>
+        <v>0.02771503092720217</v>
       </c>
       <c r="F3">
-        <v>-0.05391471495687534</v>
+        <v>-0.05556955588644442</v>
       </c>
       <c r="G3">
-        <v>-0.06253280915464397</v>
+        <v>-0.06463751991784057</v>
       </c>
       <c r="H3">
-        <v>0.1111497886989482</v>
+        <v>0.1146910281989733</v>
       </c>
       <c r="I3">
-        <v>0.06909878822468789</v>
+        <v>0.09652520864899328</v>
       </c>
       <c r="J3">
-        <v>-0.01909015669427782</v>
+        <v>-0.05239032369778457</v>
       </c>
       <c r="K3">
-        <v>-0.04374136016896989</v>
+        <v>-0.05126324650408413</v>
       </c>
       <c r="L3">
-        <v>0.006575284563791996</v>
+        <v>-0.003435706016208673</v>
       </c>
       <c r="M3">
-        <v>0.07679382384287423</v>
+        <v>0.06539098660404966</v>
       </c>
       <c r="N3">
-        <v>0.03795934618164015</v>
+        <v>0.05038073059792177</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -550,43 +550,43 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.0783303930584449</v>
+        <v>-0.1977895957625399</v>
       </c>
       <c r="C4">
-        <v>0.1221720518472285</v>
+        <v>0.1754789520186602</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.2981098520604903</v>
+        <v>0.1837602300496707</v>
       </c>
       <c r="F4">
-        <v>-0.1633195338039325</v>
+        <v>-0.1460803540235835</v>
       </c>
       <c r="G4">
-        <v>-0.1470984054862519</v>
+        <v>-0.1345222434929064</v>
       </c>
       <c r="H4">
-        <v>0.3588750911617425</v>
+        <v>0.3366930990988854</v>
       </c>
       <c r="I4">
-        <v>-0.5151684230962238</v>
+        <v>-0.3482231603619768</v>
       </c>
       <c r="J4">
-        <v>0.01043230032222128</v>
+        <v>-0.1039164003795496</v>
       </c>
       <c r="K4">
-        <v>-0.459597172319483</v>
+        <v>-0.4081009320055506</v>
       </c>
       <c r="L4">
-        <v>-0.342156576835674</v>
+        <v>-0.3005519182748715</v>
       </c>
       <c r="M4">
-        <v>0.3420214029909316</v>
+        <v>0.2776321694413547</v>
       </c>
       <c r="N4">
-        <v>-0.4634142680280373</v>
+        <v>-0.3571763908955822</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -594,43 +594,43 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-0.03052985330403633</v>
+        <v>0.00953015815020954</v>
       </c>
       <c r="C5">
-        <v>0.05653006462466296</v>
+        <v>0.02771503092720217</v>
       </c>
       <c r="D5">
-        <v>0.2981098520604903</v>
+        <v>0.1837602300496707</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.3612509639485904</v>
+        <v>0.3581846282573636</v>
       </c>
       <c r="G5">
-        <v>0.3641198327393359</v>
+        <v>0.3614420468932035</v>
       </c>
       <c r="H5">
-        <v>0.4127631093249592</v>
+        <v>0.4012543964666505</v>
       </c>
       <c r="I5">
-        <v>0.03599422413450309</v>
+        <v>0.006822339822395155</v>
       </c>
       <c r="J5">
-        <v>0.7921024341773386</v>
+        <v>0.7983442545732148</v>
       </c>
       <c r="K5">
-        <v>0.08673123342589122</v>
+        <v>0.09569588899601536</v>
       </c>
       <c r="L5">
-        <v>-0.002601885874268448</v>
+        <v>0.01011896657585113</v>
       </c>
       <c r="M5">
-        <v>0.3904627113860717</v>
+        <v>0.3944467797448968</v>
       </c>
       <c r="N5">
-        <v>-0.0004828960342666396</v>
+        <v>-0.01425156638275876</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -638,43 +638,43 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.01371389403032016</v>
+        <v>0.01584236461698259</v>
       </c>
       <c r="C6">
-        <v>-0.05391471495687534</v>
+        <v>-0.05556955588644442</v>
       </c>
       <c r="D6">
-        <v>-0.1633195338039325</v>
+        <v>-0.1460803540235835</v>
       </c>
       <c r="E6">
-        <v>0.3612509639485904</v>
+        <v>0.3581846282573636</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.9809329076610995</v>
+        <v>0.980928852548448</v>
       </c>
       <c r="H6">
-        <v>0.3722554629941501</v>
+        <v>0.3685197946180032</v>
       </c>
       <c r="I6">
-        <v>0.1806114662513572</v>
+        <v>0.1761391727802132</v>
       </c>
       <c r="J6">
-        <v>0.6301873021039683</v>
+        <v>0.6185290620948303</v>
       </c>
       <c r="K6">
-        <v>-0.04454127211874876</v>
+        <v>-0.04412919963610557</v>
       </c>
       <c r="L6">
-        <v>-0.3129315469833898</v>
+        <v>-0.3118451534525333</v>
       </c>
       <c r="M6">
-        <v>0.3725002900626034</v>
+        <v>0.3676699584686091</v>
       </c>
       <c r="N6">
-        <v>0.05618209907557382</v>
+        <v>0.05412256302001409</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -682,43 +682,43 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.0124000437774399</v>
+        <v>0.01516645206850985</v>
       </c>
       <c r="C7">
-        <v>-0.06253280915464397</v>
+        <v>-0.06463751991784057</v>
       </c>
       <c r="D7">
-        <v>-0.1470984054862519</v>
+        <v>-0.1345222434929064</v>
       </c>
       <c r="E7">
-        <v>0.3641198327393359</v>
+        <v>0.3614420468932035</v>
       </c>
       <c r="F7">
-        <v>0.9809329076610995</v>
+        <v>0.980928852548448</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.3743625636196435</v>
+        <v>0.3699904242157438</v>
       </c>
       <c r="I7">
-        <v>0.2414502345040999</v>
+        <v>0.2355494801008387</v>
       </c>
       <c r="J7">
-        <v>0.6426601479267363</v>
+        <v>0.6315276142144191</v>
       </c>
       <c r="K7">
-        <v>0.008927636603904878</v>
+        <v>0.00934476116828869</v>
       </c>
       <c r="L7">
-        <v>-0.268192419546511</v>
+        <v>-0.2677596881566871</v>
       </c>
       <c r="M7">
-        <v>0.3823050395265182</v>
+        <v>0.3769175723241422</v>
       </c>
       <c r="N7">
-        <v>0.07325264309598917</v>
+        <v>0.07066182269695842</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -726,43 +726,43 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.04819288080125357</v>
+        <v>-0.05184377338114116</v>
       </c>
       <c r="C8">
-        <v>0.1111497886989482</v>
+        <v>0.1146910281989733</v>
       </c>
       <c r="D8">
-        <v>0.3588750911617425</v>
+        <v>0.3366930990988854</v>
       </c>
       <c r="E8">
-        <v>0.4127631093249592</v>
+        <v>0.4012543964666505</v>
       </c>
       <c r="F8">
-        <v>0.3722554629941501</v>
+        <v>0.3685197946180032</v>
       </c>
       <c r="G8">
-        <v>0.3743625636196435</v>
+        <v>0.3699904242157438</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>-0.1997910261620322</v>
+        <v>-0.1889160726068343</v>
       </c>
       <c r="J8">
-        <v>0.4475614826426157</v>
+        <v>0.4271370019900166</v>
       </c>
       <c r="K8">
-        <v>-0.1437392066062044</v>
+        <v>-0.1407985109390405</v>
       </c>
       <c r="L8">
-        <v>-0.2180916373139349</v>
+        <v>-0.2086571319298562</v>
       </c>
       <c r="M8">
-        <v>0.9172288078615954</v>
+        <v>0.912656523852559</v>
       </c>
       <c r="N8">
-        <v>-0.159014452899539</v>
+        <v>-0.1531507197198079</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -770,43 +770,43 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-0.1023235157253121</v>
+        <v>-0.1409981214786789</v>
       </c>
       <c r="C9">
-        <v>0.06909878822468789</v>
+        <v>0.09652520864899328</v>
       </c>
       <c r="D9">
-        <v>-0.5151684230962238</v>
+        <v>-0.3482231603619768</v>
       </c>
       <c r="E9">
-        <v>0.03599422413450309</v>
+        <v>0.006822339822395155</v>
       </c>
       <c r="F9">
-        <v>0.1806114662513572</v>
+        <v>0.1761391727802132</v>
       </c>
       <c r="G9">
-        <v>0.2414502345040999</v>
+        <v>0.2355494801008387</v>
       </c>
       <c r="H9">
-        <v>-0.1997910261620322</v>
+        <v>-0.1889160726068343</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>0.2333820891919775</v>
+        <v>0.1892206722387704</v>
       </c>
       <c r="K9">
-        <v>0.6883971392785034</v>
+        <v>0.6643566344192655</v>
       </c>
       <c r="L9">
-        <v>0.5246616647241267</v>
+        <v>0.4960415350896452</v>
       </c>
       <c r="M9">
-        <v>-0.2193972891311861</v>
+        <v>-0.2274648898758793</v>
       </c>
       <c r="N9">
-        <v>0.7480185820308105</v>
+        <v>0.7496178209675342</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -814,43 +814,43 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-0.01461638364964552</v>
+        <v>0.03196566811971526</v>
       </c>
       <c r="C10">
-        <v>-0.01909015669427782</v>
+        <v>-0.05239032369778457</v>
       </c>
       <c r="D10">
-        <v>0.01043230032222128</v>
+        <v>-0.1039164003795496</v>
       </c>
       <c r="E10">
-        <v>0.7921024341773386</v>
+        <v>0.7983442545732148</v>
       </c>
       <c r="F10">
-        <v>0.6301873021039683</v>
+        <v>0.6185290620948303</v>
       </c>
       <c r="G10">
-        <v>0.6426601479267363</v>
+        <v>0.6315276142144191</v>
       </c>
       <c r="H10">
-        <v>0.4475614826426157</v>
+        <v>0.4271370019900166</v>
       </c>
       <c r="I10">
-        <v>0.2333820891919775</v>
+        <v>0.1892206722387704</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0.2711736763683567</v>
+        <v>0.2755031665414788</v>
       </c>
       <c r="L10">
-        <v>0.05649703490390926</v>
+        <v>0.06563921175841496</v>
       </c>
       <c r="M10">
-        <v>0.4819490113416408</v>
+        <v>0.4772401623332313</v>
       </c>
       <c r="N10">
-        <v>0.1951778656562174</v>
+        <v>0.1723205790794998</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -858,43 +858,43 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.05652648764826258</v>
+        <v>0.0665734164232875</v>
       </c>
       <c r="C11">
-        <v>-0.04374136016896989</v>
+        <v>-0.05126324650408413</v>
       </c>
       <c r="D11">
-        <v>-0.459597172319483</v>
+        <v>-0.4081009320055506</v>
       </c>
       <c r="E11">
-        <v>0.08673123342589122</v>
+        <v>0.09569588899601536</v>
       </c>
       <c r="F11">
-        <v>-0.04454127211874876</v>
+        <v>-0.04412919963610557</v>
       </c>
       <c r="G11">
-        <v>0.008927636603904878</v>
+        <v>0.00934476116828869</v>
       </c>
       <c r="H11">
-        <v>-0.1437392066062044</v>
+        <v>-0.1407985109390405</v>
       </c>
       <c r="I11">
-        <v>0.6883971392785034</v>
+        <v>0.6643566344192655</v>
       </c>
       <c r="J11">
-        <v>0.2711736763683567</v>
+        <v>0.2755031665414788</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0.931601405267243</v>
+        <v>0.9291646513948305</v>
       </c>
       <c r="M11">
-        <v>-0.13932507739623</v>
+        <v>-0.1302229061075761</v>
       </c>
       <c r="N11">
-        <v>0.759344995191208</v>
+        <v>0.7526418513922563</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -902,43 +902,43 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.02823333018647582</v>
+        <v>0.04435601442290548</v>
       </c>
       <c r="C12">
-        <v>0.006575284563791996</v>
+        <v>-0.003435706016208673</v>
       </c>
       <c r="D12">
-        <v>-0.342156576835674</v>
+        <v>-0.3005519182748715</v>
       </c>
       <c r="E12">
-        <v>-0.002601885874268448</v>
+        <v>0.01011896657585113</v>
       </c>
       <c r="F12">
-        <v>-0.3129315469833898</v>
+        <v>-0.3118451534525333</v>
       </c>
       <c r="G12">
-        <v>-0.268192419546511</v>
+        <v>-0.2677596881566871</v>
       </c>
       <c r="H12">
-        <v>-0.2180916373139349</v>
+        <v>-0.2086571319298562</v>
       </c>
       <c r="I12">
-        <v>0.5246616647241267</v>
+        <v>0.4960415350896452</v>
       </c>
       <c r="J12">
-        <v>0.05649703490390926</v>
+        <v>0.06563921175841496</v>
       </c>
       <c r="K12">
-        <v>0.931601405267243</v>
+        <v>0.9291646513948305</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>-0.2257734971776478</v>
+        <v>-0.2054599720196534</v>
       </c>
       <c r="N12">
-        <v>0.7016434961541568</v>
+        <v>0.6915138823168836</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -946,43 +946,43 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-0.03196208928288601</v>
+        <v>-0.01419361331937312</v>
       </c>
       <c r="C13">
-        <v>0.07679382384287423</v>
+        <v>0.06539098660404966</v>
       </c>
       <c r="D13">
-        <v>0.3420214029909316</v>
+        <v>0.2776321694413547</v>
       </c>
       <c r="E13">
-        <v>0.3904627113860717</v>
+        <v>0.3944467797448968</v>
       </c>
       <c r="F13">
-        <v>0.3725002900626034</v>
+        <v>0.3676699584686091</v>
       </c>
       <c r="G13">
-        <v>0.3823050395265182</v>
+        <v>0.3769175723241422</v>
       </c>
       <c r="H13">
-        <v>0.9172288078615954</v>
+        <v>0.912656523852559</v>
       </c>
       <c r="I13">
-        <v>-0.2193972891311861</v>
+        <v>-0.2274648898758793</v>
       </c>
       <c r="J13">
-        <v>0.4819490113416408</v>
+        <v>0.4772401623332313</v>
       </c>
       <c r="K13">
-        <v>-0.13932507739623</v>
+        <v>-0.1302229061075761</v>
       </c>
       <c r="L13">
-        <v>-0.2257734971776478</v>
+        <v>-0.2054599720196534</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>-0.1896858643044187</v>
+        <v>-0.1903295950547503</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -990,40 +990,40 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-0.01748914489945714</v>
+        <v>-0.03413895618995193</v>
       </c>
       <c r="C14">
-        <v>0.03795934618164015</v>
+        <v>0.05038073059792177</v>
       </c>
       <c r="D14">
-        <v>-0.4634142680280373</v>
+        <v>-0.3571763908955822</v>
       </c>
       <c r="E14">
-        <v>-0.0004828960342666396</v>
+        <v>-0.01425156638275876</v>
       </c>
       <c r="F14">
-        <v>0.05618209907557382</v>
+        <v>0.05412256302001409</v>
       </c>
       <c r="G14">
-        <v>0.07325264309598917</v>
+        <v>0.07066182269695842</v>
       </c>
       <c r="H14">
-        <v>-0.159014452899539</v>
+        <v>-0.1531507197198079</v>
       </c>
       <c r="I14">
-        <v>0.7480185820308105</v>
+        <v>0.7496178209675342</v>
       </c>
       <c r="J14">
-        <v>0.1951778656562174</v>
+        <v>0.1723205790794998</v>
       </c>
       <c r="K14">
-        <v>0.759344995191208</v>
+        <v>0.7526418513922563</v>
       </c>
       <c r="L14">
-        <v>0.7016434961541568</v>
+        <v>0.6915138823168836</v>
       </c>
       <c r="M14">
-        <v>-0.1896858643044187</v>
+        <v>-0.1903295950547503</v>
       </c>
       <c r="N14">
         <v>1</v>

</xml_diff>